<commit_message>
Corrected position servo in Wrist
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MiniBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Minibot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5820C8BF-3856-4BCE-A1D8-A888D7E6B1FA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A56915A-0308-4B6D-B4D1-B0198C896AA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Source" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="93">
   <si>
     <t>https://www.e-motionsupply.com/product_p/csf-mini.htm</t>
   </si>
@@ -152,9 +152,6 @@
     <t>https://www.kugellager-express.de/rillenkugellager-6705-2rs-61705-2rs-25x32x4-mm</t>
   </si>
   <si>
-    <t>ball bearing forearm shaft</t>
-  </si>
-  <si>
     <t>forearm shaft reenforcement</t>
   </si>
   <si>
@@ -206,20 +203,123 @@
     <t>wrist &amp; hand length</t>
   </si>
   <si>
-    <t>Screws knuckle</t>
-  </si>
-  <si>
     <t>https://www.mhm-modellbau.de/part-TT-PV0261.php</t>
   </si>
   <si>
-    <t>M2.6x14</t>
+    <t>ball bearing Forearm shaft</t>
+  </si>
+  <si>
+    <t>Gripper</t>
+  </si>
+  <si>
+    <t>Worm Shaft</t>
+  </si>
+  <si>
+    <t>Brass pipe 4mm 3mm</t>
+  </si>
+  <si>
+    <t>Worm Bearings</t>
+  </si>
+  <si>
+    <t>ball bearing 4x7x2.5</t>
+  </si>
+  <si>
+    <t>ball bearing 3x7x2</t>
+  </si>
+  <si>
+    <t>Knuckle Bearings</t>
+  </si>
+  <si>
+    <t>Shafts Gripper 9x (2mmx24mm)</t>
+  </si>
+  <si>
+    <t>Steel Shaft 2mm 250mm</t>
+  </si>
+  <si>
+    <t>Shafts Finger 3x 10x 1mmx24mm</t>
+  </si>
+  <si>
+    <t>Steel Shaft 1mm 800mm</t>
+  </si>
+  <si>
+    <t>Centre knuckle bearings</t>
+  </si>
+  <si>
+    <t>Screw knuckle</t>
+  </si>
+  <si>
+    <t>Screw Servos top</t>
+  </si>
+  <si>
+    <t>DIN 912 M2x12</t>
+  </si>
+  <si>
+    <t>Screws Top to Cover</t>
+  </si>
+  <si>
+    <t>DIN 912 M2x8</t>
+  </si>
+  <si>
+    <t>Connector Top to Body</t>
+  </si>
+  <si>
+    <t>http://www.tme.eu/de/details/tff-m2x5_dr111/distanzelemente-aus-metall/dremec/111x05/</t>
+  </si>
+  <si>
+    <t>M2 10mm hex spacer sleeve</t>
+  </si>
+  <si>
+    <t>DIN 912 M2x20</t>
+  </si>
+  <si>
+    <t>Screws Bottom to Body</t>
+  </si>
+  <si>
+    <t>Screw Servo Bottom</t>
+  </si>
+  <si>
+    <t>DIN 912 M2x10</t>
+  </si>
+  <si>
+    <t>DIN 912 M2.6x14</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>https://www.kugellager-express.de/miniatur-kugellager-683-w2-offen-3x7x2-mm</t>
+  </si>
+  <si>
+    <t>https://www.kugellager-express.de/miniatur-kugellager-mr74-zz-4x7x2-5-mm</t>
+  </si>
+  <si>
+    <t>Servo knuckle</t>
+  </si>
+  <si>
+    <t>Herkulex DRS-0101</t>
+  </si>
+  <si>
+    <t>https://www.francerobotique.com/servomoteurs-intelligents/175-herkulex-drs-0101-art0175-dst-robotpoids-45g-dimensions-45-x-24-x-32-mm-rapport-de-reduction-266-1-tension-dalimentation-7-12v-c.html</t>
+  </si>
+  <si>
+    <t>Preis</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>CAD</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="8">
+  <numFmts count="9">
+    <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="_-* #,##0.0\ _€_-;\-* #,##0.0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
@@ -229,7 +329,7 @@
     <numFmt numFmtId="169" formatCode="_-* #,##0\ _€_-;\-* #,##0\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="170" formatCode="0.000"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +360,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -278,13 +386,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -321,12 +430,19 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="4" applyFont="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Komma" xfId="1" builtinId="3"/>
     <cellStyle name="Link" xfId="3" builtinId="8"/>
     <cellStyle name="Prozent" xfId="2" builtinId="5"/>
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Währung" xfId="4" builtinId="4"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -610,17 +726,17 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="2" max="2" width="33.26171875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -628,20 +744,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" t="s">
         <v>48</v>
-      </c>
-      <c r="C3" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -651,110 +767,443 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A96A100-131C-4505-B57E-D75729258986}">
-  <dimension ref="B3:F9"/>
+  <dimension ref="A2:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="A44" sqref="A44:XFD44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="3" max="3" width="23.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.26171875" customWidth="1"/>
+    <col min="4" max="6" width="27.05078125" customWidth="1"/>
+    <col min="7" max="7" width="28" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="20" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
+        <v>65</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
-      </c>
-      <c r="E3" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B4">
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>67</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F4" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>59</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6">
         <v>2</v>
       </c>
-      <c r="C5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>37</v>
-      </c>
-      <c r="E5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C6" t="s">
+        <v>61</v>
+      </c>
+      <c r="D6" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>64</v>
       </c>
       <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
-      </c>
-      <c r="E8" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.55000000000000004">
       <c r="B9">
         <v>2</v>
       </c>
       <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B10">
+        <v>4</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>73</v>
+      </c>
+      <c r="D11" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>75</v>
+      </c>
+      <c r="D12" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E12" s="18"/>
+      <c r="F12" s="18"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>79</v>
+      </c>
+      <c r="D13" t="s">
+        <v>78</v>
+      </c>
+      <c r="H13" s="18"/>
+      <c r="I13" s="18"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B14">
+        <v>4</v>
+      </c>
+      <c r="C14" t="s">
+        <v>80</v>
+      </c>
+      <c r="D14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="14.7" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>50</v>
+      </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
         <v>57</v>
       </c>
-      <c r="D9" t="s">
-        <v>59</v>
-      </c>
-      <c r="E9" t="s">
-        <v>58</v>
+      <c r="D19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="D22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>41</v>
+      </c>
+      <c r="D23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" s="20" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="20" t="s">
+        <v>83</v>
+      </c>
+      <c r="D25" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="E25" s="20" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="H25" s="20" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B26">
+        <f>SUMIF($D$1:$D$23,D26,$B$1:$B$23)</f>
+        <v>2</v>
+      </c>
+      <c r="D26" t="s">
+        <v>62</v>
+      </c>
+      <c r="E26" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="F26" s="22">
+        <f>E26*B26</f>
+        <v>2.6</v>
+      </c>
+      <c r="G26" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B27">
+        <f>SUMIF($D$1:$D$23,D27,$B$1:$B$23)</f>
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>63</v>
+      </c>
+      <c r="E27" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="F27" s="22">
+        <f t="shared" ref="F27:F29" si="0">E27*B27</f>
+        <v>9.1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>84</v>
+      </c>
+      <c r="H27" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B28">
+        <f t="shared" ref="B28:B43" si="1">SUMIF($D$1:$D$23,D28,$B$1:$B$23)</f>
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>36</v>
+      </c>
+      <c r="E28" s="21">
+        <v>5</v>
+      </c>
+      <c r="F28" s="22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>25</v>
+      </c>
+      <c r="H28" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B29">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>37</v>
+      </c>
+      <c r="E29" s="21">
+        <v>5</v>
+      </c>
+      <c r="F29" s="22">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="G29" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D31" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="E31" s="18"/>
+      <c r="F31" s="18"/>
+      <c r="G31" s="19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B33">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D33" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B34">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B35">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="D35" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="D36" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B38">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D38" t="s">
+        <v>82</v>
+      </c>
+      <c r="G38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+      <c r="E40" s="21">
+        <v>36.9</v>
+      </c>
+      <c r="F40" s="22">
+        <f>E40*B40</f>
+        <v>73.8</v>
+      </c>
+      <c r="G40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B42">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D42" t="s">
+        <v>40</v>
+      </c>
+      <c r="G42" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="B43">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="15.6" x14ac:dyDescent="0.6">
+      <c r="F45" s="23">
+        <f>SUM(F26:F41)</f>
+        <v>100.5</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G29" r:id="rId1" xr:uid="{33221FD2-9205-4966-AFBF-E15E32492B0E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -766,25 +1215,25 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="38.7109375" customWidth="1"/>
-    <col min="3" max="3" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" customWidth="1"/>
-    <col min="6" max="6" width="11.7109375" customWidth="1"/>
-    <col min="7" max="7" width="4.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="38.68359375" customWidth="1"/>
+    <col min="3" max="3" width="13.26171875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.26171875" customWidth="1"/>
+    <col min="6" max="6" width="11.68359375" customWidth="1"/>
+    <col min="7" max="7" width="4.68359375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" customWidth="1"/>
-    <col min="12" max="12" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="18" width="9.7109375" customWidth="1"/>
-    <col min="19" max="19" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="25" max="27" width="16.28515625" customWidth="1"/>
-    <col min="32" max="32" width="32.5703125" customWidth="1"/>
+    <col min="12" max="12" width="7.41796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.41796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="18" width="9.68359375" customWidth="1"/>
+    <col min="19" max="19" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="9.578125" bestFit="1" customWidth="1"/>
+    <col min="25" max="27" width="16.26171875" customWidth="1"/>
+    <col min="32" max="32" width="32.578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" t="s">
         <v>19</v>
       </c>
@@ -798,9 +1247,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C3">
         <v>108</v>
@@ -813,9 +1262,9 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4">
         <v>167</v>
@@ -828,9 +1277,9 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C5">
         <v>0</v>
@@ -843,9 +1292,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6">
         <v>150</v>
@@ -854,9 +1303,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1">
         <v>0.5</v>
@@ -873,7 +1322,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -893,7 +1342,7 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -913,7 +1362,7 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -933,13 +1382,13 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="G11" s="1">
         <f>SUM(G7:G10)</f>
         <v>4.3</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -948,7 +1397,7 @@
       </c>
       <c r="D12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -959,7 +1408,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -971,14 +1420,14 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -998,7 +1447,7 @@
         <v>5.1257250000000001</v>
       </c>
     </row>
-    <row r="18" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1018,7 +1467,7 @@
         <v>11.600325000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1487,7 @@
         <v>6.6349935000000002</v>
       </c>
     </row>
-    <row r="20" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1058,9 +1507,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C21" s="1">
         <f>((C6)*(C10+C7)*($C$14))/1000</f>
@@ -1078,9 +1527,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1">
         <f>((C6)*(C7)*($C$14))/1000</f>
@@ -1098,17 +1547,17 @@
         <v>3.9240000000000004E-3</v>
       </c>
     </row>
-    <row r="23" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
     </row>
-    <row r="24" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C24" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D24" s="1"/>
     </row>
-    <row r="25" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -1125,7 +1574,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="26" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1591,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -1159,7 +1608,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="G28" s="4"/>
@@ -1188,7 +1637,7 @@
       <c r="AD28" s="4"/>
       <c r="AE28" s="4"/>
     </row>
-    <row r="29" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1223,7 +1672,7 @@
       <c r="S29" s="4"/>
       <c r="T29" s="4"/>
     </row>
-    <row r="30" spans="1:39" ht="45" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:39" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1264,7 +1713,7 @@
       <c r="Z30" s="9"/>
       <c r="AA30" s="9"/>
     </row>
-    <row r="31" spans="1:39" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:39" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1305,7 +1754,7 @@
       <c r="Z31" s="9"/>
       <c r="AA31" s="9"/>
     </row>
-    <row r="32" spans="1:39" ht="17.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:39" ht="17.5" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="F32" s="5"/>
@@ -1339,7 +1788,7 @@
       <c r="AL32" s="4"/>
       <c r="AM32" s="4"/>
     </row>
-    <row r="33" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="F33" s="5"/>
@@ -1376,7 +1825,7 @@
       <c r="AL33" s="4"/>
       <c r="AM33" s="4"/>
     </row>
-    <row r="34" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="F34" s="5"/>
@@ -1413,7 +1862,7 @@
       <c r="AL34" s="4"/>
       <c r="AM34" s="4"/>
     </row>
-    <row r="35" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="F35" s="13"/>
@@ -1451,7 +1900,7 @@
       <c r="AL35" s="4"/>
       <c r="AM35" s="4"/>
     </row>
-    <row r="36" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C36" s="16"/>
       <c r="E36" s="6"/>
       <c r="F36" s="6"/>
@@ -1470,7 +1919,7 @@
       <c r="T36" s="14"/>
       <c r="X36" s="1"/>
     </row>
-    <row r="37" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C37" s="16"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
@@ -1489,56 +1938,56 @@
       <c r="T37" s="14"/>
       <c r="X37" s="1"/>
     </row>
-    <row r="38" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="16"/>
     </row>
-    <row r="39" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
     </row>
-    <row r="40" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
     </row>
-    <row r="41" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
     </row>
-    <row r="42" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
     </row>
-    <row r="45" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C45" s="17"/>
       <c r="D45" s="17"/>
     </row>
-    <row r="46" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C46" s="17"/>
       <c r="D46" s="17"/>
     </row>
-    <row r="47" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C47" s="17"/>
       <c r="D47" s="17"/>
       <c r="F47" s="17"/>
     </row>
-    <row r="48" spans="3:39" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:39" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" s="17"/>
       <c r="D48" s="17"/>
     </row>
-    <row r="49" spans="3:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:4" ht="22.9" customHeight="1" x14ac:dyDescent="0.55000000000000004"/>
+    <row r="51" spans="3:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C51" s="17"/>
       <c r="D51" s="17"/>
     </row>
-    <row r="52" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C52" s="17"/>
       <c r="D52" s="17"/>
     </row>
-    <row r="53" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C53" s="17"/>
       <c r="D53" s="17"/>
     </row>
-    <row r="54" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:4" x14ac:dyDescent="0.55000000000000004">
       <c r="C54" s="17"/>
       <c r="D54" s="17"/>
     </row>

</xml_diff>

<commit_message>
made new Elbow main strand
</commit_message>
<xml_diff>
--- a/bom.xlsx
+++ b/bom.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jochen Alt\Documents\Daten\Projects\MiniBot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\MiniBot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FF1EEB7-81A2-481F-90C2-0F047408C14C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DF93287-0708-45BE-82BF-C37BCFCC6638}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="23235" windowHeight="12555" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="168">
   <si>
     <t>https://www.e-motionsupply.com/product_p/csf-mini.htm</t>
   </si>
@@ -522,6 +522,15 @@
   </si>
   <si>
     <t>Steel Rod 1x500mm</t>
+  </si>
+  <si>
+    <t>UART Connector Odroid C2-Herkulex Servos</t>
+  </si>
+  <si>
+    <t>4-channel bidirectional level shifter</t>
+  </si>
+  <si>
+    <t>https://www.ebay.de/itm/4-Kanal-Pegelwandler-I2C-5V-3-3V-Level-Shifter-Konverter-Arduino-Raspberry-Pi/252742078456?hash=item3ad89a0ff8:g:pKkAAOSwCK1b6qwj</t>
   </si>
 </sst>
 </file>
@@ -979,10 +988,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A96A100-131C-4505-B57E-D75729258986}">
-  <dimension ref="A2:L116"/>
+  <dimension ref="A2:L118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:XFD5"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="J115" sqref="J115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1017,7 @@
         <v>160</v>
       </c>
       <c r="D3" t="str">
-        <f>D110</f>
+        <f>D111</f>
         <v>Steel Rod 2x500mm</v>
       </c>
     </row>
@@ -1020,7 +1029,7 @@
         <v>163</v>
       </c>
       <c r="D4" t="str">
-        <f>D111</f>
+        <f>D112</f>
         <v>Steel Rod 1x500mm</v>
       </c>
     </row>
@@ -1070,7 +1079,7 @@
         <v>59</v>
       </c>
       <c r="D10" t="str">
-        <f>D80</f>
+        <f>D81</f>
         <v>ball bearing 4x7x2.5</v>
       </c>
     </row>
@@ -1082,7 +1091,7 @@
         <v>62</v>
       </c>
       <c r="D11" t="str">
-        <f>D81</f>
+        <f>D82</f>
         <v>ball bearing 3x7x2</v>
       </c>
     </row>
@@ -1094,7 +1103,7 @@
         <v>67</v>
       </c>
       <c r="D12" t="str">
-        <f>D81</f>
+        <f>D82</f>
         <v>ball bearing 3x7x2</v>
       </c>
     </row>
@@ -1106,7 +1115,7 @@
         <v>68</v>
       </c>
       <c r="D13" t="str">
-        <f>D98</f>
+        <f>D99</f>
         <v>DIN 912 M2.6x14</v>
       </c>
     </row>
@@ -1180,7 +1189,7 @@
         <v>84</v>
       </c>
       <c r="D19" t="str">
-        <f>D100</f>
+        <f>D101</f>
         <v>Herkulex DRS-0101</v>
       </c>
     </row>
@@ -1192,7 +1201,7 @@
         <v>112</v>
       </c>
       <c r="D20" t="str">
-        <f>D101</f>
+        <f>D102</f>
         <v>Herkulex DRS-0201</v>
       </c>
     </row>
@@ -1215,7 +1224,7 @@
         <v>94</v>
       </c>
       <c r="D23" t="str">
-        <f>D83</f>
+        <f>D84</f>
         <v>ball bearing 25x32x4</v>
       </c>
     </row>
@@ -1227,7 +1236,7 @@
         <v>93</v>
       </c>
       <c r="D24" t="str">
-        <f>D82</f>
+        <f>D83</f>
         <v>ball bearing 20x27x4</v>
       </c>
     </row>
@@ -1239,7 +1248,7 @@
         <v>96</v>
       </c>
       <c r="D25" t="str">
-        <f>D89</f>
+        <f>D90</f>
         <v>DIN 912 M2x6</v>
       </c>
     </row>
@@ -1252,7 +1261,7 @@
         <v>98</v>
       </c>
       <c r="D26" t="str">
-        <f>D90</f>
+        <f>D91</f>
         <v>DIN 912 M2x8</v>
       </c>
     </row>
@@ -1264,7 +1273,7 @@
         <v>100</v>
       </c>
       <c r="D27" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1276,7 +1285,7 @@
         <v>101</v>
       </c>
       <c r="D28" t="str">
-        <f>D85</f>
+        <f>D86</f>
         <v xml:space="preserve">M2 10mm hex spacer </v>
       </c>
     </row>
@@ -1288,7 +1297,7 @@
         <v>26</v>
       </c>
       <c r="D29" t="str">
-        <f>D81</f>
+        <f>D82</f>
         <v>ball bearing 3x7x2</v>
       </c>
     </row>
@@ -1300,7 +1309,7 @@
         <v>49</v>
       </c>
       <c r="D30" t="str">
-        <f>D82</f>
+        <f>D83</f>
         <v>ball bearing 20x27x4</v>
       </c>
     </row>
@@ -1312,7 +1321,7 @@
         <v>56</v>
       </c>
       <c r="D31" t="str">
-        <f>D83</f>
+        <f>D84</f>
         <v>ball bearing 25x32x4</v>
       </c>
     </row>
@@ -1324,7 +1333,7 @@
         <v>113</v>
       </c>
       <c r="D32" t="str">
-        <f>D102</f>
+        <f>D103</f>
         <v>Herkulex DRS-0401</v>
       </c>
     </row>
@@ -1341,7 +1350,7 @@
         <v>98</v>
       </c>
       <c r="D35" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1353,7 +1362,7 @@
         <v>115</v>
       </c>
       <c r="D36" t="str">
-        <f>D93</f>
+        <f>D94</f>
         <v>DIN 912 M2x16</v>
       </c>
     </row>
@@ -1365,7 +1374,7 @@
         <v>116</v>
       </c>
       <c r="D37" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1377,7 +1386,7 @@
         <v>116</v>
       </c>
       <c r="D38" t="str">
-        <f>D96</f>
+        <f>D97</f>
         <v>DIN 912 M2x30</v>
       </c>
     </row>
@@ -1405,7 +1414,7 @@
         <v>120</v>
       </c>
       <c r="D43" t="str">
-        <f>D109</f>
+        <f>D110</f>
         <v>M2 threaded rod 500mm</v>
       </c>
     </row>
@@ -1417,7 +1426,7 @@
         <v>121</v>
       </c>
       <c r="D44" t="str">
-        <f>D83</f>
+        <f>D84</f>
         <v>ball bearing 25x32x4</v>
       </c>
     </row>
@@ -1434,7 +1443,7 @@
         <v>123</v>
       </c>
       <c r="D47" t="str">
-        <f>D101</f>
+        <f>D102</f>
         <v>Herkulex DRS-0201</v>
       </c>
     </row>
@@ -1446,7 +1455,7 @@
         <v>124</v>
       </c>
       <c r="D48" t="str">
-        <f>D105</f>
+        <f>D106</f>
         <v>Herkulex DRS-0602</v>
       </c>
     </row>
@@ -1458,7 +1467,7 @@
         <v>125</v>
       </c>
       <c r="D49" t="str">
-        <f>D90</f>
+        <f>D91</f>
         <v>DIN 912 M2x8</v>
       </c>
     </row>
@@ -1470,7 +1479,7 @@
         <v>126</v>
       </c>
       <c r="D50" t="str">
-        <f>D96</f>
+        <f>D97</f>
         <v>DIN 912 M2x30</v>
       </c>
     </row>
@@ -1482,7 +1491,7 @@
         <v>128</v>
       </c>
       <c r="D51" t="str">
-        <f>D85</f>
+        <f>D86</f>
         <v xml:space="preserve">M2 10mm hex spacer </v>
       </c>
     </row>
@@ -1497,7 +1506,7 @@
         <v>135</v>
       </c>
       <c r="D53" t="str">
-        <f>D82</f>
+        <f>D83</f>
         <v>ball bearing 20x27x4</v>
       </c>
     </row>
@@ -1509,7 +1518,7 @@
         <v>136</v>
       </c>
       <c r="D54" t="str">
-        <f>D102</f>
+        <f>D103</f>
         <v>Herkulex DRS-0401</v>
       </c>
     </row>
@@ -1521,7 +1530,7 @@
         <v>137</v>
       </c>
       <c r="D55" t="str">
-        <f>D95</f>
+        <f>D96</f>
         <v>DIN 912 M2x25</v>
       </c>
     </row>
@@ -1533,7 +1542,7 @@
         <v>139</v>
       </c>
       <c r="D56" t="str">
-        <f>D93</f>
+        <f>D94</f>
         <v>DIN 912 M2x16</v>
       </c>
     </row>
@@ -1545,7 +1554,7 @@
         <v>126</v>
       </c>
       <c r="D57" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1557,7 +1566,7 @@
         <v>140</v>
       </c>
       <c r="D58" t="str">
-        <f>D91</f>
+        <f>D92</f>
         <v>DIN 912 M2x10</v>
       </c>
     </row>
@@ -1569,7 +1578,7 @@
         <v>101</v>
       </c>
       <c r="D59" t="str">
-        <f>D85</f>
+        <f>D86</f>
         <v xml:space="preserve">M2 10mm hex spacer </v>
       </c>
     </row>
@@ -1586,7 +1595,7 @@
         <v>113</v>
       </c>
       <c r="D62" t="str">
-        <f>D102</f>
+        <f>D103</f>
         <v>Herkulex DRS-0401</v>
       </c>
     </row>
@@ -1598,7 +1607,7 @@
         <v>147</v>
       </c>
       <c r="D63" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1610,7 +1619,7 @@
         <v>126</v>
       </c>
       <c r="D64" t="str">
-        <f>D91</f>
+        <f>D92</f>
         <v>DIN 912 M2x10</v>
       </c>
     </row>
@@ -1622,7 +1631,7 @@
         <v>145</v>
       </c>
       <c r="D65" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1634,7 +1643,7 @@
         <v>148</v>
       </c>
       <c r="D66" t="str">
-        <f>D85</f>
+        <f>D86</f>
         <v xml:space="preserve">M2 10mm hex spacer </v>
       </c>
     </row>
@@ -1646,7 +1655,7 @@
         <v>149</v>
       </c>
       <c r="D67" t="str">
-        <f>D91</f>
+        <f>D92</f>
         <v>DIN 912 M2x10</v>
       </c>
     </row>
@@ -1658,7 +1667,7 @@
         <v>151</v>
       </c>
       <c r="D68" t="str">
-        <f>D84</f>
+        <f>D85</f>
         <v>ball bearing 65x85x10</v>
       </c>
     </row>
@@ -1670,7 +1679,7 @@
         <v>152</v>
       </c>
       <c r="D69" t="str">
-        <f>D109</f>
+        <f>D110</f>
         <v>M2 threaded rod 500mm</v>
       </c>
     </row>
@@ -1687,7 +1696,7 @@
         <v>142</v>
       </c>
       <c r="D71" t="str">
-        <f>D112</f>
+        <f>D113</f>
         <v>Hohlbuchse 5.5/2.1mm</v>
       </c>
     </row>
@@ -1699,7 +1708,7 @@
         <v>125</v>
       </c>
       <c r="D72" t="str">
-        <f>D91</f>
+        <f>D92</f>
         <v>DIN 912 M2x10</v>
       </c>
     </row>
@@ -1711,7 +1720,7 @@
         <v>145</v>
       </c>
       <c r="D73" t="str">
-        <f>D94</f>
+        <f>D95</f>
         <v>DIN 912 M2x20</v>
       </c>
     </row>
@@ -1729,7 +1738,7 @@
         <v>158</v>
       </c>
       <c r="D76" t="str">
-        <f>D114</f>
+        <f>D115</f>
         <v>Odroid C2</v>
       </c>
     </row>
@@ -1741,111 +1750,93 @@
         <v>156</v>
       </c>
       <c r="D77" t="str">
-        <f>D113</f>
+        <f>D114</f>
         <v>Step down Voltage regulator 5V 2A</v>
       </c>
     </row>
-    <row r="79" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="20" t="s">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="B78">
+        <v>1</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78" t="str">
+        <f>D116</f>
+        <v>4-channel bidirectional level shifter</v>
+      </c>
+    </row>
+    <row r="80" spans="1:11" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A80" s="20" t="s">
         <v>81</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="D80" s="20" t="s">
         <v>88</v>
       </c>
-      <c r="E79" s="20" t="s">
+      <c r="E80" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="H79" s="20" t="s">
+      <c r="H80" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="I79" s="20" t="s">
+      <c r="I80" s="20" t="s">
         <v>103</v>
       </c>
-      <c r="J79" s="20" t="s">
+      <c r="J80" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="K79" s="20" t="s">
+      <c r="K80" s="20" t="s">
         <v>90</v>
-      </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B80">
-        <f>SUMIF($D$1:$D$72,D80,$B$1:$B$72)</f>
-        <v>2</v>
-      </c>
-      <c r="D80" t="s">
-        <v>60</v>
-      </c>
-      <c r="E80" s="21">
-        <v>1.3</v>
-      </c>
-      <c r="F80" s="22">
-        <f>E80*B80</f>
-        <v>2.6</v>
-      </c>
-      <c r="G80" s="22"/>
-      <c r="H80" s="22"/>
-      <c r="I80" s="24">
-        <f t="shared" ref="I80:I81" si="0">IF(B80-H80&gt;=0,B80-H80,0)</f>
-        <v>2</v>
-      </c>
-      <c r="J80" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="81" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B81">
-        <f>SUMIF($D$1:$D$72,D81,$B$1:$B$72)</f>
-        <v>7</v>
+        <f t="shared" ref="B81:B97" si="0">SUMIF($D$1:$D$72,D81,$B$1:$B$72)</f>
+        <v>2</v>
       </c>
       <c r="D81" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E81" s="21">
         <v>1.3</v>
       </c>
       <c r="F81" s="22">
-        <f t="shared" ref="F81:F83" si="1">E81*B81</f>
-        <v>9.1</v>
+        <f>E81*B81</f>
+        <v>2.6</v>
       </c>
       <c r="G81" s="22"/>
       <c r="H81" s="22"/>
       <c r="I81" s="24">
+        <f t="shared" ref="I81:I82" si="1">IF(B81-H81&gt;=0,B81-H81,0)</f>
+        <v>2</v>
+      </c>
+      <c r="J81" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B82">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="J81" t="s">
+      <c r="D82" t="s">
+        <v>61</v>
+      </c>
+      <c r="E82" s="21">
+        <v>1.3</v>
+      </c>
+      <c r="F82" s="22">
+        <f t="shared" ref="F82:F84" si="2">E82*B82</f>
+        <v>9.1</v>
+      </c>
+      <c r="G82" s="22"/>
+      <c r="H82" s="22"/>
+      <c r="I82" s="24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="J82" t="s">
         <v>82</v>
-      </c>
-      <c r="K81" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="82" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B82">
-        <f>SUMIF($D$1:$D$72,D82,$B$1:$B$72)</f>
-        <v>3</v>
-      </c>
-      <c r="D82" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" s="21">
-        <v>5</v>
-      </c>
-      <c r="F82" s="22">
-        <f t="shared" si="1"/>
-        <v>15</v>
-      </c>
-      <c r="G82" s="22"/>
-      <c r="H82" s="24">
-        <v>3</v>
-      </c>
-      <c r="I82" s="24">
-        <f>IF(B82-H82&gt;=0,B82-H82,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J82" t="s">
-        <v>25</v>
       </c>
       <c r="K82" t="s">
         <v>27</v>
@@ -1853,253 +1844,253 @@
     </row>
     <row r="83" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B83">
-        <f>SUMIF($D$1:$D$72,D83,$B$1:$B$72)</f>
-        <v>5</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="D83" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E83" s="21">
         <v>5</v>
       </c>
       <c r="F83" s="22">
-        <f t="shared" si="1"/>
-        <v>25</v>
+        <f t="shared" si="2"/>
+        <v>15</v>
       </c>
       <c r="G83" s="22"/>
       <c r="H83" s="24">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I83" s="24">
         <f>IF(B83-H83&gt;=0,B83-H83,0)</f>
-        <v>3</v>
-      </c>
-      <c r="J83" s="19" t="s">
-        <v>38</v>
+        <v>0</v>
+      </c>
+      <c r="J83" t="s">
+        <v>25</v>
+      </c>
+      <c r="K83" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="84" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B84">
-        <f>SUMIF($D$1:$D$72,D84,$B$1:$B$72)</f>
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D84" t="s">
+        <v>37</v>
+      </c>
+      <c r="E84" s="21">
+        <v>5</v>
+      </c>
+      <c r="F84" s="22">
+        <f t="shared" si="2"/>
+        <v>25</v>
+      </c>
+      <c r="G84" s="22"/>
+      <c r="H84" s="24">
         <v>2</v>
       </c>
-      <c r="D84" t="s">
-        <v>150</v>
+      <c r="I84" s="24">
+        <f>IF(B84-H84&gt;=0,B84-H84,0)</f>
+        <v>3</v>
+      </c>
+      <c r="J84" s="19" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="85" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B85">
-        <f>SUMIF($D$1:$D$72,D85,$B$1:$B$72)</f>
-        <v>27</v>
-      </c>
-      <c r="D85" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="E85" s="18"/>
-      <c r="F85" s="18"/>
-      <c r="G85" s="18"/>
-      <c r="H85" s="18">
-        <v>10</v>
-      </c>
-      <c r="I85" s="24">
-        <f>IF(B85-H85&gt;=0,B85-H85,0)</f>
-        <v>17</v>
-      </c>
-      <c r="J85" s="19" t="s">
-        <v>74</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D85" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="86" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B86">
-        <f>SUMIF($D$1:$D$72,D86,$B$1:$B$72)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>27</v>
       </c>
       <c r="D86" s="25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E86" s="18"/>
       <c r="F86" s="18"/>
       <c r="G86" s="18"/>
       <c r="H86" s="18">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I86" s="24">
         <f>IF(B86-H86&gt;=0,B86-H86,0)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
       <c r="J86" s="19" t="s">
-        <v>129</v>
+        <v>74</v>
       </c>
     </row>
     <row r="87" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B87">
-        <f>SUMIF($D$1:$D$72,D87,$B$1:$B$72)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="D87" s="25" t="s">
-        <v>131</v>
+        <v>133</v>
+      </c>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="18"/>
+      <c r="H87" s="18">
+        <v>0</v>
+      </c>
+      <c r="I87" s="24">
+        <f>IF(B87-H87&gt;=0,B87-H87,0)</f>
+        <v>0</v>
       </c>
       <c r="J87" s="19" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="88" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B88">
-        <f>SUMIF($D$1:$D$72,D88,$B$1:$B$72)</f>
-        <v>0</v>
-      </c>
-      <c r="D88" t="s">
-        <v>95</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="D88" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="J88" s="19" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B89">
-        <f>SUMIF($D$1:$D$72,D89,$B$1:$B$72)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D89" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="90" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B90">
-        <f>SUMIF($D$1:$D$72,D90,$B$1:$B$72)</f>
-        <v>20</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="D90" t="s">
-        <v>72</v>
+        <v>97</v>
       </c>
     </row>
     <row r="91" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B91">
-        <f>SUMIF($D$1:$D$72,D91,$B$1:$B$72)</f>
-        <v>32</v>
+        <f t="shared" si="0"/>
+        <v>20</v>
       </c>
       <c r="D91" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
     </row>
     <row r="92" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B92">
-        <f>SUMIF($D$1:$D$72,D92,$B$1:$B$72)</f>
-        <v>7</v>
+        <f t="shared" si="0"/>
+        <v>32</v>
       </c>
       <c r="D92" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B93">
-        <f>SUMIF($D$1:$D$72,D93,$B$1:$B$72)</f>
-        <v>8</v>
+        <f t="shared" si="0"/>
+        <v>7</v>
       </c>
       <c r="D93" t="s">
-        <v>99</v>
+        <v>70</v>
       </c>
     </row>
     <row r="94" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B94">
-        <f>SUMIF($D$1:$D$72,D94,$B$1:$B$72)</f>
-        <v>29</v>
+        <f t="shared" si="0"/>
+        <v>8</v>
       </c>
       <c r="D94" t="s">
-        <v>76</v>
+        <v>99</v>
       </c>
     </row>
     <row r="95" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B95">
-        <f>SUMIF($D$1:$D$72,D95,$B$1:$B$72)</f>
-        <v>4</v>
+        <f t="shared" si="0"/>
+        <v>29</v>
       </c>
       <c r="D95" t="s">
-        <v>138</v>
+        <v>76</v>
       </c>
     </row>
     <row r="96" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B96">
-        <f>SUMIF($D$1:$D$72,D96,$B$1:$B$72)</f>
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D96" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="97" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B97">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="D96" t="s">
+      <c r="D97" t="s">
         <v>117</v>
       </c>
-      <c r="J96" t="s">
+      <c r="J97" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="98" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B98">
-        <f>SUMIF($D$1:$D$72,D98,$B$1:$B$72)</f>
+    <row r="99" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B99">
+        <f>SUMIF($D$1:$D$72,D99,$B$1:$B$72)</f>
         <v>2</v>
       </c>
-      <c r="D98" t="s">
+      <c r="D99" t="s">
         <v>80</v>
       </c>
-      <c r="H98">
+      <c r="H99">
         <v>10</v>
       </c>
-      <c r="I98" s="24">
-        <f>IF(B98-H98&gt;=0,B98-H98,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J98" t="s">
+      <c r="I99" s="24">
+        <f>IF(B99-H99&gt;=0,B99-H99,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J99" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="100" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B100">
-        <f>SUMIF($D$1:$D$72,D100,$B$1:$B$72)</f>
-        <v>1</v>
-      </c>
-      <c r="D100" t="s">
-        <v>85</v>
-      </c>
-      <c r="E100" s="21">
-        <v>36.9</v>
-      </c>
-      <c r="F100" s="22">
-        <f t="shared" ref="F100:F105" si="2">E100*B100</f>
-        <v>36.9</v>
-      </c>
-      <c r="G100" s="22">
-        <f>I100*E100</f>
-        <v>0</v>
-      </c>
-      <c r="H100" s="24">
-        <v>5</v>
-      </c>
-      <c r="I100" s="24">
-        <f>IF(B100-H100&gt;=0,B100-H100,0)</f>
-        <v>0</v>
-      </c>
-      <c r="J100" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="101" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B101">
-        <f>SUMIF($D$1:$D$72,D101,$B$1:$B$72)</f>
-        <v>2</v>
+        <f t="shared" ref="B101:B106" si="3">SUMIF($D$1:$D$72,D101,$B$1:$B$72)</f>
+        <v>1</v>
       </c>
       <c r="D101" t="s">
-        <v>104</v>
+        <v>85</v>
       </c>
       <c r="E101" s="21">
         <v>36.9</v>
       </c>
       <c r="F101" s="22">
-        <f t="shared" si="2"/>
-        <v>73.8</v>
+        <f t="shared" ref="F101:F106" si="4">E101*B101</f>
+        <v>36.9</v>
       </c>
       <c r="G101" s="22">
-        <f t="shared" ref="G101:G105" si="3">I101*E101</f>
+        <f>I101*E101</f>
         <v>0</v>
       </c>
       <c r="H101" s="24">
         <v>5</v>
       </c>
       <c r="I101" s="24">
-        <f t="shared" ref="I101:I114" si="4">IF(B101-H101&gt;=0,B101-H101,0)</f>
+        <f>IF(B101-H101&gt;=0,B101-H101,0)</f>
         <v>0</v>
       </c>
       <c r="J101" t="s">
@@ -2108,28 +2099,28 @@
     </row>
     <row r="102" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B102">
-        <f>SUMIF($D$1:$D$72,D102,$B$1:$B$72)</f>
-        <v>4</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="D102" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E102" s="21">
-        <v>250</v>
+        <v>36.9</v>
       </c>
       <c r="F102" s="22">
-        <f t="shared" si="2"/>
-        <v>1000</v>
+        <f t="shared" si="4"/>
+        <v>73.8</v>
       </c>
       <c r="G102" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="G102:G106" si="5">I102*E102</f>
         <v>0</v>
       </c>
       <c r="H102" s="24">
         <v>5</v>
       </c>
       <c r="I102" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="I102:I115" si="6">IF(B102-H102&gt;=0,B102-H102,0)</f>
         <v>0</v>
       </c>
       <c r="J102" t="s">
@@ -2138,256 +2129,316 @@
     </row>
     <row r="103" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B103">
-        <f>SUMIF($D$1:$D$72,D103,$B$1:$B$72)</f>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>4</v>
       </c>
       <c r="D103" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E103" s="21">
-        <v>222</v>
+        <v>250</v>
       </c>
       <c r="F103" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="4"/>
+        <v>1000</v>
       </c>
       <c r="G103" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-      <c r="H103" s="24"/>
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H103" s="24">
+        <v>5</v>
+      </c>
       <c r="I103" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J103" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
     </row>
     <row r="104" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B104">
-        <f>SUMIF($D$1:$D$72,D104,$B$1:$B$72)</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="D104" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E104" s="21">
-        <v>250</v>
+        <v>222</v>
       </c>
       <c r="F104" s="22">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="G104" s="22">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>0</v>
       </c>
       <c r="H104" s="24"/>
       <c r="I104" s="24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="J104" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="105" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B105">
-        <f>SUMIF($D$1:$D$72,D105,$B$1:$B$72)</f>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>0</v>
       </c>
       <c r="D105" t="s">
+        <v>108</v>
+      </c>
+      <c r="E105" s="21">
+        <v>250</v>
+      </c>
+      <c r="F105" s="22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G105" s="22">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J105" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B106">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="D106" t="s">
         <v>109</v>
       </c>
-      <c r="E105" s="21">
+      <c r="E106" s="21">
         <v>300</v>
       </c>
-      <c r="F105" s="22">
-        <f t="shared" si="2"/>
+      <c r="F106" s="22">
+        <f t="shared" si="4"/>
         <v>300</v>
       </c>
-      <c r="G105" s="22">
-        <f t="shared" si="3"/>
+      <c r="G106" s="22">
+        <f t="shared" si="5"/>
         <v>300</v>
       </c>
-      <c r="H105" s="24">
-        <v>0</v>
-      </c>
-      <c r="I105" s="24">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J105" t="s">
+      <c r="H106" s="24">
+        <v>0</v>
+      </c>
+      <c r="I106" s="24">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J106" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="106" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="H106" s="24">
-        <v>0</v>
-      </c>
-      <c r="I106" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
     <row r="107" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B107">
-        <f>SUMIF($D$1:$D$72,D107,$B$1:$B$72)</f>
-        <v>1</v>
-      </c>
-      <c r="D107" t="s">
-        <v>40</v>
-      </c>
       <c r="H107" s="24">
         <v>0</v>
       </c>
       <c r="I107" s="24">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J107" t="s">
-        <v>35</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
       </c>
     </row>
     <row r="108" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B108">
-        <f>SUMIF($D$1:$D$72,D108,$B$1:$B$72)</f>
-        <v>0</v>
+        <f t="shared" ref="B108:B115" si="7">SUMIF($D$1:$D$72,D108,$B$1:$B$72)</f>
+        <v>1</v>
       </c>
       <c r="D108" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H108" s="24">
         <v>0</v>
       </c>
       <c r="I108" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="J108" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
     </row>
     <row r="109" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B109">
-        <f>SUMIF($D$1:$D$72,D109,$B$1:$B$72)</f>
-        <v>2</v>
+        <f t="shared" si="7"/>
+        <v>0</v>
       </c>
       <c r="D109" t="s">
-        <v>119</v>
+        <v>41</v>
       </c>
       <c r="H109" s="24">
         <v>0</v>
       </c>
       <c r="I109" s="24">
-        <f t="shared" si="4"/>
-        <v>2</v>
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J109" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="110" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B110">
-        <f>SUMIF($D$1:$D$72,D110,$B$1:$B$72)</f>
-        <v>1</v>
+        <f t="shared" si="7"/>
+        <v>2</v>
       </c>
       <c r="D110" t="s">
-        <v>161</v>
-      </c>
-      <c r="H110" s="24"/>
-      <c r="I110" s="24"/>
+        <v>119</v>
+      </c>
+      <c r="H110" s="24">
+        <v>0</v>
+      </c>
+      <c r="I110" s="24">
+        <f t="shared" si="6"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="111" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B111">
-        <f>SUMIF($D$1:$D$72,D111,$B$1:$B$72)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D111" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="H111" s="24"/>
       <c r="I111" s="24"/>
     </row>
     <row r="112" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B112">
-        <f>SUMIF($D$1:$D$72,D112,$B$1:$B$72)</f>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="D112" t="s">
-        <v>144</v>
-      </c>
-      <c r="H112" s="24">
-        <v>0</v>
-      </c>
-      <c r="I112" s="24">
-        <f t="shared" si="4"/>
-        <v>1</v>
-      </c>
-      <c r="J112" t="s">
-        <v>143</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="H112" s="24"/>
+      <c r="I112" s="24"/>
     </row>
     <row r="113" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B113">
-        <f>SUMIF($D$1:$D$72,D113,$B$1:$B$72)</f>
-        <v>0</v>
+        <f t="shared" si="7"/>
+        <v>1</v>
       </c>
       <c r="D113" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="H113" s="24">
         <v>0</v>
       </c>
       <c r="I113" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
+        <f t="shared" si="6"/>
+        <v>1</v>
       </c>
       <c r="J113" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
     </row>
     <row r="114" spans="2:10" x14ac:dyDescent="0.25">
       <c r="B114">
-        <f>SUMIF($D$1:$D$72,D114,$B$1:$B$72)</f>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="D114" t="s">
+        <v>155</v>
+      </c>
+      <c r="H114" s="24">
+        <v>0</v>
+      </c>
+      <c r="I114" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="J114" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="115" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B115">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="D115" t="s">
         <v>157</v>
       </c>
-      <c r="E114" s="21">
+      <c r="E115" s="21">
         <v>59</v>
       </c>
-      <c r="F114" s="22">
-        <f t="shared" ref="F114" si="5">E114*B114</f>
-        <v>0</v>
-      </c>
-      <c r="G114" s="22">
-        <f t="shared" ref="G114" si="6">I114*E114</f>
-        <v>0</v>
-      </c>
-      <c r="H114" s="24">
-        <v>1</v>
-      </c>
-      <c r="I114" s="24">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="F116" s="23">
-        <f>SUM(F80:F106)</f>
+      <c r="F115" s="22">
+        <f t="shared" ref="F115" si="8">E115*B115</f>
+        <v>0</v>
+      </c>
+      <c r="G115" s="22">
+        <f t="shared" ref="G115" si="9">I115*E115</f>
+        <v>0</v>
+      </c>
+      <c r="H115" s="24">
+        <v>1</v>
+      </c>
+      <c r="I115" s="24">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B116">
+        <f t="shared" ref="B116" si="10">SUMIF($D$1:$D$72,D116,$B$1:$B$72)</f>
+        <v>0</v>
+      </c>
+      <c r="D116" t="s">
+        <v>166</v>
+      </c>
+      <c r="E116" s="21">
+        <v>2.5</v>
+      </c>
+      <c r="F116" s="22">
+        <f t="shared" ref="F116" si="11">E116*B116</f>
+        <v>0</v>
+      </c>
+      <c r="G116" s="22">
+        <f t="shared" ref="G116" si="12">I116*E116</f>
+        <v>0</v>
+      </c>
+      <c r="H116" s="24">
+        <v>1</v>
+      </c>
+      <c r="I116" s="24">
+        <f t="shared" ref="I116" si="13">IF(B116-H116&gt;=0,B116-H116,0)</f>
+        <v>0</v>
+      </c>
+      <c r="J116" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="118" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="F118" s="23">
+        <f>SUM(F81:F107)</f>
         <v>1462.4</v>
       </c>
-      <c r="G116" s="23">
-        <f>SUM(G80:G106)</f>
+      <c r="G118" s="23">
+        <f>SUM(G81:G107)</f>
         <v>300</v>
       </c>
-      <c r="H116" s="23"/>
-      <c r="I116" s="23"/>
+      <c r="H118" s="23"/>
+      <c r="I118" s="23"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J83" r:id="rId1" xr:uid="{33221FD2-9205-4966-AFBF-E15E32492B0E}"/>
-    <hyperlink ref="J87" r:id="rId2" xr:uid="{C148C300-CD23-4055-A158-AC5493D7815A}"/>
+    <hyperlink ref="J84" r:id="rId1" xr:uid="{33221FD2-9205-4966-AFBF-E15E32492B0E}"/>
+    <hyperlink ref="J88" r:id="rId2" xr:uid="{C148C300-CD23-4055-A158-AC5493D7815A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>

</xml_diff>